<commit_message>
update total workforce numbers for canada
</commit_message>
<xml_diff>
--- a/Livelihoods/Employment_Figures/Raw files/Canada/Community Labour Force Activity, 1986 to 2014.xlsx
+++ b/Livelihoods/Employment_Figures/Raw files/Canada/Community Labour Force Activity, 1986 to 2014.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="792" windowWidth="25440" windowHeight="15996" tabRatio="554" activeTab="4"/>
+    <workbookView xWindow="2280" yWindow="792" windowWidth="25440" windowHeight="15996" tabRatio="554"/>
   </bookViews>
   <sheets>
     <sheet name="2014" sheetId="17" r:id="rId1"/>
@@ -27,7 +27,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="10">'1986'!$1:$5</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1327,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N164"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -5906,7 +5906,7 @@
   <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -7526,7 +7526,7 @@
   <dimension ref="A1:R71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="12" x14ac:dyDescent="0.25"/>
@@ -9174,7 +9174,7 @@
   <dimension ref="A1:K69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="11.4" x14ac:dyDescent="0.2"/>
@@ -10757,8 +10757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12" x14ac:dyDescent="0.25"/>

</xml_diff>